<commit_message>
new board top/bottom pdf's on 11x17
</commit_message>
<xml_diff>
--- a/LEVER-bom.xlsx
+++ b/LEVER-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>Part name</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>http://katalog.we-online.de/pbs/datasheet/750032050.pdf</t>
+  </si>
+  <si>
+    <t>Mike's actual List:</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,6 +694,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -855,10 +864,13 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1202,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A39" sqref="A38:A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,10 +1255,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2">
@@ -1266,10 +1278,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C3">
@@ -1289,10 +1301,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C4">
@@ -1315,10 +1327,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C5">
@@ -1338,10 +1350,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C6">
@@ -1361,10 +1373,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C7">
@@ -1384,10 +1396,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C8">
@@ -1409,160 +1421,162 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1625</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>938</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>356</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C16">
@@ -1571,7 +1585,7 @@
       <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F16" t="s">
@@ -1579,7 +1593,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1883,6 +1897,11 @@
       </c>
       <c r="G31" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1900,8 +1919,9 @@
     <hyperlink ref="D15" r:id="rId11"/>
     <hyperlink ref="D9" r:id="rId12"/>
     <hyperlink ref="D10" r:id="rId13"/>
+    <hyperlink ref="E16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>